<commit_message>
upload excel file in order to creating units
</commit_message>
<xml_diff>
--- a/app/units.xlsx
+++ b/app/units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alitabatabaeiat/Documents/Dev/NodeJs/Final project backend/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51980FC7-2926-904C-8F9F-F4D4735F7A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0926BD6D-1252-4A42-8A2F-1185A0E6C496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1081,7 +1081,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>